<commit_message>
pacing modes & relevant fields
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -379,6 +379,46 @@
           <t>Password</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Lower Rate Limit</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Upper Rate Limit</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Atrial Amplitude</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Atrial Pulse Width</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Ventricular Amplitude</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Ventricular Pulse Width</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>VRP</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>ARP</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -404,6 +444,33 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>ben</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>john</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>doe</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test@test.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>johndoe</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>test</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented writing to spreadsheet on save on mainPage
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -44,15 +44,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,7 +474,46 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I commited this issue because im having trouble fixing it, if someone could help me fix it ill be able to zoom through the rest of this.
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -446,6 +446,11 @@
           <t>ben</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">

</xml_diff>

<commit_message>
issue with storing and pulling resolved
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -477,8 +477,45 @@
           <t>test</t>
         </is>
       </c>
-      <c r="F3" t="n">
-        <v>120</v>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -539,14 +576,37 @@
           <t>test</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>12</v>
-      </c>
-      <c r="G5" t="n">
-        <v>13</v>
-      </c>
-      <c r="H5" t="n">
-        <v>14</v>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented incorrect login message.
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="16240" windowWidth="28800" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -43,15 +43,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -549,6 +549,41 @@
           <t>120</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>1231</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -591,13 +626,11 @@
           <t>1</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>0</t>
@@ -610,6 +643,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Parameters can now only take on certain ranges
</commit_message>
<xml_diff>
--- a/userdata.xlsx
+++ b/userdata.xlsx
@@ -68,7 +68,10 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -380,352 +383,332 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E11" activeCellId="0" pane="topLeft" sqref="A11:E11"/>
+      <selection activeCell="E16" activeCellId="0" pane="topLeft" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5390625" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="1">
-      <c r="A1" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="1" s="2">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>First name</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Last name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Username</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Password</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>Lower Rate Limit</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Upper Rate Limit</t>
         </is>
       </c>
-      <c r="H1" s="2" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>Atrial Amplitude</t>
         </is>
       </c>
-      <c r="I1" s="2" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>Atrial Pulse Width</t>
         </is>
       </c>
-      <c r="J1" s="2" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>Ventricular Amplitude</t>
         </is>
       </c>
-      <c r="K1" s="2" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>Ventricular Pulse Width</t>
         </is>
       </c>
-      <c r="L1" s="2" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>VRP</t>
         </is>
       </c>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>ARP</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="2" s="1">
-      <c r="A2" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="2" s="2">
+      <c r="A2" s="3" t="inlineStr">
         <is>
           <t>alksjdlaksjd</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>lkjaslk;djlk;</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>jlkasjdlk;ajsdl</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>kjslkdjalkdsjalk</t>
         </is>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="3" t="inlineStr">
         <is>
           <t>jlksjdaklsjda</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="3" s="1">
-      <c r="A3" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="3" s="2">
+      <c r="A3" s="3" t="inlineStr">
         <is>
           <t>askjdaksljdlkj</t>
         </is>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>lkjsadlkjaskldj</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>kljsadkjjdlaksjd</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>aslkdjaklsjd</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="3" t="inlineStr">
         <is>
           <t>aslkdjaskl</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="4" s="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
+    <row customHeight="1" ht="15" r="4" s="2">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>sd</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>aa</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="5" s="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="5" s="2">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>asddd</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="6" s="1">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="6" s="2">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>sd</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>assss</t>
         </is>
       </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="7" s="1">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="15" r="7" s="2">
+      <c r="A7" s="3" t="inlineStr">
         <is>
           <t>asdasdasdasd</t>
         </is>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>asasdasd</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>sadasdasd</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>asdasdasd</t>
         </is>
       </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t>sasdsa</t>
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15" r="8" s="1">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>asdasdas</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>sasasad</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>dsadsadadsa</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>sdadsad</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="inlineStr">
-        <is>
-          <t>dasadasasd</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="9" s="1">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>asdasdads</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>dsadasdsads</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>dsasdda</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>sdasdsadasd</t>
-        </is>
-      </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>asdasdasdasdsd</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="15" r="10" s="1">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>adasdsadas</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>sadasdas</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>sadasdasd</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>asdsadsadsasad</t>
-        </is>
-      </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>dsasadsadsad</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="11" s="1">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>sdfjasdklf;j</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>jjasklsjda;slkdj</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>l;kjsklajkldjalk</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>jksajdl;kasjdkl</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>jlk;jsadalkjdaslkdj</t>
-        </is>
-      </c>
-    </row>
-    <row customHeight="1" ht="13.8" r="12" s="1"/>
-    <row customHeight="1" ht="13.8" r="13" s="1"/>
-    <row customHeight="1" ht="13.8" r="14" s="1"/>
-    <row customHeight="1" ht="13.8" r="15" s="1"/>
+    <row customHeight="1" ht="15" r="8" s="2">
+      <c r="A8" s="3" t="n"/>
+      <c r="B8" s="3" t="n"/>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n"/>
+      <c r="E8" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="9" s="2">
+      <c r="A9" s="3" t="n"/>
+      <c r="B9" s="3" t="n"/>
+      <c r="C9" s="3" t="n"/>
+      <c r="D9" s="3" t="n"/>
+      <c r="E9" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="10" s="2">
+      <c r="A10" s="3" t="n"/>
+      <c r="B10" s="3" t="n"/>
+      <c r="C10" s="3" t="n"/>
+      <c r="D10" s="3" t="n"/>
+      <c r="E10" s="3" t="n"/>
+    </row>
+    <row customHeight="1" ht="13.8" r="11" s="2">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>uday</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>uday</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>uday</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>uday</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>uday</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H11" s="3" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="I11" s="3" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>0.5</t>
+        </is>
+      </c>
+      <c r="K11" s="3" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="L11" s="3" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="M11" s="3" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+    </row>
+    <row customHeight="1" ht="13.8" r="12" s="2"/>
+    <row customHeight="1" ht="13.8" r="13" s="2"/>
+    <row customHeight="1" ht="13.8" r="14" s="2"/>
+    <row customHeight="1" ht="13.8" r="15" s="2"/>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>

</xml_diff>